<commit_message>
v2.0.4 add date check
</commit_message>
<xml_diff>
--- a/Duty/Список проживающих.xlsx
+++ b/Duty/Список проживающих.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Bot\Duty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCA04BE-9F4D-4679-A55F-5337E02F4E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D183FDB4-79CF-4810-848D-251FF3CD12BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,7 +764,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,19 +789,20 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -828,9 +829,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -838,6 +838,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1154,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,7 +1728,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B72">
@@ -1816,7 +1818,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B84">
@@ -1832,7 +1834,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B86">
@@ -1965,7 +1967,7 @@
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2007,7 +2009,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B109">
@@ -2060,10 +2062,10 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B116" s="4">
         <v>192062697</v>
       </c>
     </row>
@@ -2076,7 +2078,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B118">
@@ -2230,7 +2232,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B138">
@@ -2297,7 +2299,7 @@
       <c r="A146" t="s">
         <v>146</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2321,7 +2323,7 @@
       <c r="A149" t="s">
         <v>150</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2400,7 +2402,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B160">
@@ -2435,7 +2437,7 @@
       <c r="A164" t="s">
         <v>166</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2480,7 +2482,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="7" t="s">
         <v>173</v>
       </c>
       <c r="B170">
@@ -2488,7 +2490,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="7" t="s">
         <v>174</v>
       </c>
       <c r="B171">
@@ -2544,8 +2546,11 @@
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="7" t="s">
         <v>181</v>
+      </c>
+      <c r="B178" s="6">
+        <v>135945403</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -2608,7 +2613,7 @@
       <c r="A186" t="s">
         <v>189</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="3" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2645,7 +2650,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B191">
@@ -2693,7 +2698,7 @@
       <c r="A197" t="s">
         <v>201</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B197" s="3" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2858,7 +2863,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="2" t="s">
+      <c r="A218" s="7" t="s">
         <v>223</v>
       </c>
       <c r="B218">
@@ -3023,7 +3028,7 @@
       <c r="A239" t="s">
         <v>243</v>
       </c>
-      <c r="B239" s="6">
+      <c r="B239" s="5">
         <v>157833436</v>
       </c>
     </row>
@@ -3039,7 +3044,7 @@
       <c r="A241" t="s">
         <v>245</v>
       </c>
-      <c r="B241" s="6">
+      <c r="B241" s="5">
         <v>100302835</v>
       </c>
     </row>

</xml_diff>